<commit_message>
Add: Add observations to main data
</commit_message>
<xml_diff>
--- a/JakobGregersen_NamePrediction/Maries_navne.xlsx
+++ b/JakobGregersen_NamePrediction/Maries_navne.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JakobFaarbaekGregers\Github\MachineLearning\JakobGregersen_NamePrediction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72509F76-67BF-411D-92BD-4E5E42851E3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CC56ACC-8E71-4685-B7F6-322FDC0A744F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{3B372328-9E67-3B4D-9D2E-9BC42CB3E9D8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3B372328-9E67-3B4D-9D2E-9BC42CB3E9D8}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="72">
   <si>
     <t>Navn2</t>
   </si>
@@ -92,9 +92,6 @@
     <t>*</t>
   </si>
   <si>
-    <t>false</t>
-  </si>
-  <si>
     <t>Mads</t>
   </si>
   <si>
@@ -107,9 +104,6 @@
     <t>Adam</t>
   </si>
   <si>
-    <t>true</t>
-  </si>
-  <si>
     <t>Klaes</t>
   </si>
   <si>
@@ -261,6 +255,24 @@
   </si>
   <si>
     <t>Gode_Navne1</t>
+  </si>
+  <si>
+    <t>Anker</t>
+  </si>
+  <si>
+    <t>Jon</t>
+  </si>
+  <si>
+    <t>Bo</t>
+  </si>
+  <si>
+    <t>Immanuel</t>
+  </si>
+  <si>
+    <t>Hugo</t>
+  </si>
+  <si>
+    <t>Børge</t>
   </si>
 </sst>
 </file>
@@ -453,8 +465,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E303D2DD-0BAD-9249-9574-5437E9C0A8F5}" name="Data_matricen" displayName="Data_matricen" ref="A1:H28" totalsRowShown="0" headerRowDxfId="6">
-  <autoFilter ref="A1:H28" xr:uid="{E303D2DD-0BAD-9249-9574-5437E9C0A8F5}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E303D2DD-0BAD-9249-9574-5437E9C0A8F5}" name="Data_matricen" displayName="Data_matricen" ref="A1:H31" totalsRowShown="0" headerRowDxfId="6">
+  <autoFilter ref="A1:H31" xr:uid="{E303D2DD-0BAD-9249-9574-5437E9C0A8F5}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{676840D5-3AFB-F24A-A649-95BA9D806245}" name="Navn1"/>
     <tableColumn id="2" xr3:uid="{C53193AA-DC5B-CE4B-B62E-59090314002E}" name="Navn2"/>
@@ -788,10 +800,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17EB9BB6-FC87-A044-A614-C3992330C11E}">
-  <dimension ref="A1:H28"/>
+  <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -852,103 +864,103 @@
         <f>LEFT(Data_matricen[[#This Row],[Navn2]],1)</f>
         <v>M</v>
       </c>
-      <c r="G2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H2" t="s">
-        <v>11</v>
+      <c r="G2" t="b">
+        <v>0</v>
+      </c>
+      <c r="H2" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>66</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>67</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E3" t="str">
         <f>UPPER(RIGHT(Data_matricen[[#This Row],[Navn1]],1))</f>
-        <v>S</v>
+        <v>R</v>
       </c>
       <c r="F3" t="str">
         <f>LEFT(Data_matricen[[#This Row],[Navn2]],1)</f>
-        <v>T</v>
-      </c>
-      <c r="G3" t="s">
-        <v>11</v>
-      </c>
-      <c r="H3" t="s">
-        <v>11</v>
+        <v>J</v>
+      </c>
+      <c r="G3" t="b">
+        <v>1</v>
+      </c>
+      <c r="H3" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>68</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>69</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E4" t="str">
         <f>UPPER(RIGHT(Data_matricen[[#This Row],[Navn1]],1))</f>
-        <v>S</v>
+        <v>O</v>
       </c>
       <c r="F4" t="str">
         <f>LEFT(Data_matricen[[#This Row],[Navn2]],1)</f>
-        <v>A</v>
-      </c>
-      <c r="G4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H4" t="s">
-        <v>16</v>
+        <v>I</v>
+      </c>
+      <c r="G4" t="b">
+        <v>1</v>
+      </c>
+      <c r="H4" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>70</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>71</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E5" t="str">
         <f>UPPER(RIGHT(Data_matricen[[#This Row],[Navn1]],1))</f>
-        <v>S</v>
+        <v>O</v>
       </c>
       <c r="F5" t="str">
         <f>LEFT(Data_matricen[[#This Row],[Navn2]],1)</f>
-        <v>E</v>
-      </c>
-      <c r="G5" t="s">
-        <v>11</v>
-      </c>
-      <c r="H5" t="s">
-        <v>11</v>
+        <v>B</v>
+      </c>
+      <c r="G5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H5" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -958,221 +970,221 @@
       </c>
       <c r="E6" t="str">
         <f>UPPER(RIGHT(Data_matricen[[#This Row],[Navn1]],1))</f>
-        <v>E</v>
+        <v>S</v>
       </c>
       <c r="F6" t="str">
         <f>LEFT(Data_matricen[[#This Row],[Navn2]],1)</f>
-        <v>K</v>
-      </c>
-      <c r="G6" t="s">
-        <v>11</v>
-      </c>
-      <c r="H6" t="s">
-        <v>11</v>
+        <v>T</v>
+      </c>
+      <c r="G6" t="b">
+        <v>0</v>
+      </c>
+      <c r="H6" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="C7">
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E7" t="str">
         <f>UPPER(RIGHT(Data_matricen[[#This Row],[Navn1]],1))</f>
-        <v>D</v>
+        <v>S</v>
       </c>
       <c r="F7" t="str">
         <f>LEFT(Data_matricen[[#This Row],[Navn2]],1)</f>
-        <v>F</v>
-      </c>
-      <c r="G7" t="s">
-        <v>11</v>
-      </c>
-      <c r="H7" t="s">
-        <v>16</v>
+        <v>A</v>
+      </c>
+      <c r="G7" t="b">
+        <v>0</v>
+      </c>
+      <c r="H7" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="B8" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="C8">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E8" t="str">
         <f>UPPER(RIGHT(Data_matricen[[#This Row],[Navn1]],1))</f>
-        <v>K</v>
+        <v>S</v>
       </c>
       <c r="F8" t="str">
         <f>LEFT(Data_matricen[[#This Row],[Navn2]],1)</f>
-        <v>W</v>
-      </c>
-      <c r="G8" t="s">
-        <v>11</v>
-      </c>
-      <c r="H8" t="s">
-        <v>11</v>
+        <v>E</v>
+      </c>
+      <c r="G8" t="b">
+        <v>0</v>
+      </c>
+      <c r="H8" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B9" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="C9">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E9" t="str">
         <f>UPPER(RIGHT(Data_matricen[[#This Row],[Navn1]],1))</f>
-        <v>R</v>
+        <v>E</v>
       </c>
       <c r="F9" t="str">
         <f>LEFT(Data_matricen[[#This Row],[Navn2]],1)</f>
-        <v>A</v>
-      </c>
-      <c r="G9" t="s">
-        <v>11</v>
-      </c>
-      <c r="H9" t="s">
-        <v>11</v>
+        <v>K</v>
+      </c>
+      <c r="G9" t="b">
+        <v>0</v>
+      </c>
+      <c r="H9" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="B10" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="C10">
-        <v>1</v>
+        <v>-2</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E10" t="str">
         <f>UPPER(RIGHT(Data_matricen[[#This Row],[Navn1]],1))</f>
-        <v>P</v>
+        <v>D</v>
       </c>
       <c r="F10" t="str">
         <f>LEFT(Data_matricen[[#This Row],[Navn2]],1)</f>
-        <v>A</v>
-      </c>
-      <c r="G10" t="s">
-        <v>11</v>
-      </c>
-      <c r="H10" t="s">
-        <v>11</v>
+        <v>F</v>
+      </c>
+      <c r="G10" t="b">
+        <v>0</v>
+      </c>
+      <c r="H10" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="B11" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="C11">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E11" t="str">
         <f>UPPER(RIGHT(Data_matricen[[#This Row],[Navn1]],1))</f>
-        <v>B</v>
+        <v>K</v>
       </c>
       <c r="F11" t="str">
         <f>LEFT(Data_matricen[[#This Row],[Navn2]],1)</f>
-        <v>F</v>
-      </c>
-      <c r="G11" t="s">
-        <v>11</v>
-      </c>
-      <c r="H11" t="s">
-        <v>11</v>
+        <v>W</v>
+      </c>
+      <c r="G11" t="b">
+        <v>0</v>
+      </c>
+      <c r="H11" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="B12" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="C12">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E12" t="str">
         <f>UPPER(RIGHT(Data_matricen[[#This Row],[Navn1]],1))</f>
-        <v>K</v>
+        <v>R</v>
       </c>
       <c r="F12" t="str">
         <f>LEFT(Data_matricen[[#This Row],[Navn2]],1)</f>
-        <v>Ø</v>
-      </c>
-      <c r="G12" t="s">
-        <v>11</v>
-      </c>
-      <c r="H12" t="s">
-        <v>16</v>
+        <v>A</v>
+      </c>
+      <c r="G12" t="b">
+        <v>0</v>
+      </c>
+      <c r="H12" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="B13" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="C13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E13" t="str">
         <f>UPPER(RIGHT(Data_matricen[[#This Row],[Navn1]],1))</f>
-        <v>F</v>
+        <v>P</v>
       </c>
       <c r="F13" t="str">
         <f>LEFT(Data_matricen[[#This Row],[Navn2]],1)</f>
-        <v>M</v>
-      </c>
-      <c r="G13" t="s">
-        <v>11</v>
-      </c>
-      <c r="H13" t="s">
-        <v>11</v>
+        <v>A</v>
+      </c>
+      <c r="G13" t="b">
+        <v>0</v>
+      </c>
+      <c r="H13" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="B14" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="C14">
         <v>0</v>
@@ -1182,53 +1194,53 @@
       </c>
       <c r="E14" t="str">
         <f>UPPER(RIGHT(Data_matricen[[#This Row],[Navn1]],1))</f>
-        <v>R</v>
+        <v>B</v>
       </c>
       <c r="F14" t="str">
         <f>LEFT(Data_matricen[[#This Row],[Navn2]],1)</f>
-        <v>H</v>
-      </c>
-      <c r="G14" t="s">
-        <v>11</v>
-      </c>
-      <c r="H14" t="s">
-        <v>16</v>
+        <v>F</v>
+      </c>
+      <c r="G14" t="b">
+        <v>0</v>
+      </c>
+      <c r="H14" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="B15" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="C15">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E15" t="str">
         <f>UPPER(RIGHT(Data_matricen[[#This Row],[Navn1]],1))</f>
-        <v>N</v>
+        <v>K</v>
       </c>
       <c r="F15" t="str">
         <f>LEFT(Data_matricen[[#This Row],[Navn2]],1)</f>
-        <v>R</v>
-      </c>
-      <c r="G15" t="s">
-        <v>16</v>
-      </c>
-      <c r="H15" t="s">
-        <v>16</v>
+        <v>Ø</v>
+      </c>
+      <c r="G15" t="b">
+        <v>0</v>
+      </c>
+      <c r="H15" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="B16" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="C16">
         <v>0</v>
@@ -1238,25 +1250,25 @@
       </c>
       <c r="E16" t="str">
         <f>UPPER(RIGHT(Data_matricen[[#This Row],[Navn1]],1))</f>
-        <v>S</v>
+        <v>F</v>
       </c>
       <c r="F16" t="str">
         <f>LEFT(Data_matricen[[#This Row],[Navn2]],1)</f>
-        <v>A</v>
-      </c>
-      <c r="G16" t="s">
-        <v>11</v>
-      </c>
-      <c r="H16" t="s">
-        <v>11</v>
+        <v>M</v>
+      </c>
+      <c r="G16" t="b">
+        <v>0</v>
+      </c>
+      <c r="H16" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="B17" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="C17">
         <v>0</v>
@@ -1266,28 +1278,28 @@
       </c>
       <c r="E17" t="str">
         <f>UPPER(RIGHT(Data_matricen[[#This Row],[Navn1]],1))</f>
-        <v>T</v>
+        <v>R</v>
       </c>
       <c r="F17" t="str">
         <f>LEFT(Data_matricen[[#This Row],[Navn2]],1)</f>
-        <v>J</v>
-      </c>
-      <c r="G17" t="s">
-        <v>16</v>
-      </c>
-      <c r="H17" t="s">
-        <v>11</v>
+        <v>H</v>
+      </c>
+      <c r="G17" t="b">
+        <v>0</v>
+      </c>
+      <c r="H17" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B18" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="C18">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>10</v>
@@ -1298,21 +1310,21 @@
       </c>
       <c r="F18" t="str">
         <f>LEFT(Data_matricen[[#This Row],[Navn2]],1)</f>
-        <v>A</v>
-      </c>
-      <c r="G18" t="s">
-        <v>11</v>
-      </c>
-      <c r="H18" t="s">
-        <v>16</v>
+        <v>R</v>
+      </c>
+      <c r="G18" t="b">
+        <v>1</v>
+      </c>
+      <c r="H18" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="B19" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="C19">
         <v>0</v>
@@ -1322,81 +1334,81 @@
       </c>
       <c r="E19" t="str">
         <f>UPPER(RIGHT(Data_matricen[[#This Row],[Navn1]],1))</f>
-        <v>N</v>
+        <v>S</v>
       </c>
       <c r="F19" t="str">
         <f>LEFT(Data_matricen[[#This Row],[Navn2]],1)</f>
-        <v>Q</v>
-      </c>
-      <c r="G19" t="s">
-        <v>11</v>
-      </c>
-      <c r="H19" t="s">
-        <v>11</v>
+        <v>A</v>
+      </c>
+      <c r="G19" t="b">
+        <v>0</v>
+      </c>
+      <c r="H19" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="B20" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="C20">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>49</v>
+        <v>10</v>
       </c>
       <c r="E20" t="str">
         <f>UPPER(RIGHT(Data_matricen[[#This Row],[Navn1]],1))</f>
-        <v>Y</v>
+        <v>T</v>
       </c>
       <c r="F20" t="str">
         <f>LEFT(Data_matricen[[#This Row],[Navn2]],1)</f>
-        <v>M</v>
-      </c>
-      <c r="G20" t="s">
-        <v>11</v>
-      </c>
-      <c r="H20" t="s">
-        <v>11</v>
+        <v>J</v>
+      </c>
+      <c r="G20" t="b">
+        <v>1</v>
+      </c>
+      <c r="H20" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="B21" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="C21">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E21" t="str">
         <f>UPPER(RIGHT(Data_matricen[[#This Row],[Navn1]],1))</f>
-        <v>D</v>
+        <v>N</v>
       </c>
       <c r="F21" t="str">
         <f>LEFT(Data_matricen[[#This Row],[Navn2]],1)</f>
-        <v>O</v>
-      </c>
-      <c r="G21" t="s">
-        <v>16</v>
-      </c>
-      <c r="H21" t="s">
-        <v>16</v>
+        <v>A</v>
+      </c>
+      <c r="G21" t="b">
+        <v>0</v>
+      </c>
+      <c r="H21" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="B22" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="C22">
         <v>0</v>
@@ -1406,185 +1418,269 @@
       </c>
       <c r="E22" t="str">
         <f>UPPER(RIGHT(Data_matricen[[#This Row],[Navn1]],1))</f>
-        <v>E</v>
+        <v>N</v>
       </c>
       <c r="F22" t="str">
         <f>LEFT(Data_matricen[[#This Row],[Navn2]],1)</f>
-        <v>M</v>
-      </c>
-      <c r="G22" t="s">
-        <v>11</v>
-      </c>
-      <c r="H22" t="s">
-        <v>11</v>
+        <v>Q</v>
+      </c>
+      <c r="G22" t="b">
+        <v>0</v>
+      </c>
+      <c r="H22" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="B23" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="C23">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>10</v>
+        <v>47</v>
       </c>
       <c r="E23" t="str">
         <f>UPPER(RIGHT(Data_matricen[[#This Row],[Navn1]],1))</f>
-        <v>F</v>
+        <v>Y</v>
       </c>
       <c r="F23" t="str">
         <f>LEFT(Data_matricen[[#This Row],[Navn2]],1)</f>
-        <v>A</v>
-      </c>
-      <c r="G23" t="s">
-        <v>11</v>
-      </c>
-      <c r="H23" t="s">
-        <v>11</v>
+        <v>M</v>
+      </c>
+      <c r="G23" t="b">
+        <v>0</v>
+      </c>
+      <c r="H23" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="B24" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="C24">
-        <v>-2</v>
+        <v>1</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E24" t="str">
         <f>UPPER(RIGHT(Data_matricen[[#This Row],[Navn1]],1))</f>
-        <v>N</v>
+        <v>D</v>
       </c>
       <c r="F24" t="str">
         <f>LEFT(Data_matricen[[#This Row],[Navn2]],1)</f>
-        <v>D</v>
-      </c>
-      <c r="G24" t="s">
-        <v>11</v>
-      </c>
-      <c r="H24" t="s">
-        <v>11</v>
+        <v>O</v>
+      </c>
+      <c r="G24" t="b">
+        <v>1</v>
+      </c>
+      <c r="H24" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="B25" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="C25">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E25" t="str">
         <f>UPPER(RIGHT(Data_matricen[[#This Row],[Navn1]],1))</f>
-        <v>T</v>
+        <v>E</v>
       </c>
       <c r="F25" t="str">
         <f>LEFT(Data_matricen[[#This Row],[Navn2]],1)</f>
-        <v>T</v>
-      </c>
-      <c r="G25" t="s">
-        <v>11</v>
-      </c>
-      <c r="H25" t="s">
-        <v>11</v>
+        <v>M</v>
+      </c>
+      <c r="G25" t="b">
+        <v>0</v>
+      </c>
+      <c r="H25" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="B26" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="C26">
-        <v>3.5</v>
+        <v>1</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E26" t="str">
         <f>UPPER(RIGHT(Data_matricen[[#This Row],[Navn1]],1))</f>
-        <v>N</v>
+        <v>F</v>
       </c>
       <c r="F26" t="str">
         <f>LEFT(Data_matricen[[#This Row],[Navn2]],1)</f>
-        <v>M</v>
-      </c>
-      <c r="G26" t="s">
-        <v>11</v>
-      </c>
-      <c r="H26" t="s">
-        <v>11</v>
+        <v>A</v>
+      </c>
+      <c r="G26" t="b">
+        <v>0</v>
+      </c>
+      <c r="H26" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="B27" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="C27">
-        <v>4</v>
+        <v>-2</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E27" t="str">
         <f>UPPER(RIGHT(Data_matricen[[#This Row],[Navn1]],1))</f>
-        <v>Y</v>
+        <v>N</v>
       </c>
       <c r="F27" t="str">
         <f>LEFT(Data_matricen[[#This Row],[Navn2]],1)</f>
-        <v>H</v>
-      </c>
-      <c r="G27" t="s">
-        <v>16</v>
-      </c>
-      <c r="H27" t="s">
-        <v>16</v>
+        <v>D</v>
+      </c>
+      <c r="G27" t="b">
+        <v>0</v>
+      </c>
+      <c r="H27" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="B28" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="C28">
+        <v>3</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E28" t="str">
+        <f>UPPER(RIGHT(Data_matricen[[#This Row],[Navn1]],1))</f>
+        <v>T</v>
+      </c>
+      <c r="F28" t="str">
+        <f>LEFT(Data_matricen[[#This Row],[Navn2]],1)</f>
+        <v>T</v>
+      </c>
+      <c r="G28" t="b">
+        <v>0</v>
+      </c>
+      <c r="H28" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>58</v>
+      </c>
+      <c r="B29" t="s">
+        <v>59</v>
+      </c>
+      <c r="C29">
+        <v>3.5</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E29" t="str">
+        <f>UPPER(RIGHT(Data_matricen[[#This Row],[Navn1]],1))</f>
+        <v>N</v>
+      </c>
+      <c r="F29" t="str">
+        <f>LEFT(Data_matricen[[#This Row],[Navn2]],1)</f>
+        <v>M</v>
+      </c>
+      <c r="G29" t="b">
+        <v>0</v>
+      </c>
+      <c r="H29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>60</v>
+      </c>
+      <c r="B30" t="s">
+        <v>61</v>
+      </c>
+      <c r="C30">
+        <v>4</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E30" t="str">
+        <f>UPPER(RIGHT(Data_matricen[[#This Row],[Navn1]],1))</f>
+        <v>Y</v>
+      </c>
+      <c r="F30" t="str">
+        <f>LEFT(Data_matricen[[#This Row],[Navn2]],1)</f>
+        <v>H</v>
+      </c>
+      <c r="G30" t="b">
+        <v>1</v>
+      </c>
+      <c r="H30" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>62</v>
+      </c>
+      <c r="B31" t="s">
+        <v>63</v>
+      </c>
+      <c r="C31">
         <v>5</v>
       </c>
-      <c r="D28" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E28" t="str">
+      <c r="D31" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E31" t="str">
         <f>UPPER(RIGHT(Data_matricen[[#This Row],[Navn1]],1))</f>
         <v>K</v>
       </c>
-      <c r="F28" t="str">
+      <c r="F31" t="str">
         <f>LEFT(Data_matricen[[#This Row],[Navn2]],1)</f>
         <v>R</v>
       </c>
-      <c r="G28" t="s">
-        <v>16</v>
-      </c>
-      <c r="H28" t="s">
-        <v>16</v>
+      <c r="G31" t="b">
+        <v>1</v>
+      </c>
+      <c r="H31" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1611,22 +1707,22 @@
   <sheetData>
     <row r="1" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D2" s="4" t="str" cm="1">
+      <c r="D2" s="4" t="e" cm="1">
         <f t="array" ref="D2">INDEX(Data_matricen[Navn1],MATCH("true",Data_matricen[Navn1_godt?],0),0)</f>
-        <v>Bjørn</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D3" s="4" t="str" cm="1">
+      <c r="D3" s="4" t="e" cm="1">
         <f t="array" ref="D3">INDEX(Data_matricen[Navn1],MATCH("true",Data_matricen[Navn1_godt?],0),0)</f>
-        <v>Bjørn</v>
+        <v>#N/A</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
chore: change capitalization of booleans
</commit_message>
<xml_diff>
--- a/JakobGregersen_NamePrediction/Maries_navne.xlsx
+++ b/JakobGregersen_NamePrediction/Maries_navne.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JakobFaarbaekGregers\Github\MachineLearning\JakobGregersen_NamePrediction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CC56ACC-8E71-4685-B7F6-322FDC0A744F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D2DB3C5-4957-4639-A3DC-8A48D10C0369}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3B372328-9E67-3B4D-9D2E-9BC42CB3E9D8}"/>
+    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{3B372328-9E67-3B4D-9D2E-9BC42CB3E9D8}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -803,7 +803,7 @@
   <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E40" sqref="E40"/>
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
chore: add poul erling
</commit_message>
<xml_diff>
--- a/JakobGregersen_NamePrediction/Maries_navne.xlsx
+++ b/JakobGregersen_NamePrediction/Maries_navne.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jakobfaarbaekgregersen/Documents/GitHub/MachineLearning/JakobGregersen_NamePrediction/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lille\Github\MachineLearning\JakobGregersen_NamePrediction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A45D1A2-7A19-6F46-BA0B-1AF23904F37D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4920161-A911-4B15-990B-886A77ECB0E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="27320" windowHeight="13860" xr2:uid="{3B372328-9E67-3B4D-9D2E-9BC42CB3E9D8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3B372328-9E67-3B4D-9D2E-9BC42CB3E9D8}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="103">
   <si>
     <t>Navn2</t>
   </si>
@@ -341,6 +341,9 @@
   </si>
   <si>
     <t>Bent</t>
+  </si>
+  <si>
+    <t>Erling</t>
   </si>
 </sst>
 </file>
@@ -429,8 +432,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E303D2DD-0BAD-9249-9574-5437E9C0A8F5}" name="Data_matricen" displayName="Data_matricen" ref="A1:H52" totalsRowShown="0" headerRowDxfId="1">
-  <autoFilter ref="A1:H52" xr:uid="{E303D2DD-0BAD-9249-9574-5437E9C0A8F5}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E303D2DD-0BAD-9249-9574-5437E9C0A8F5}" name="Data_matricen" displayName="Data_matricen" ref="A1:H53" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="A1:H53" xr:uid="{E303D2DD-0BAD-9249-9574-5437E9C0A8F5}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H43">
     <sortCondition descending="1" ref="C1:C43"/>
   </sortState>
@@ -745,24 +748,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17EB9BB6-FC87-A044-A614-C3992330C11E}">
-  <dimension ref="A1:H52"/>
+  <dimension ref="A1:H53"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A33" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A53" sqref="A53"/>
+      <selection activeCell="D53" sqref="D53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="9.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.5" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="17.125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -788,7 +791,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>63</v>
       </c>
@@ -816,7 +819,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>65</v>
       </c>
@@ -844,7 +847,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>67</v>
       </c>
@@ -872,7 +875,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>61</v>
       </c>
@@ -900,7 +903,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>34</v>
       </c>
@@ -928,7 +931,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>44</v>
       </c>
@@ -956,7 +959,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>59</v>
       </c>
@@ -984,7 +987,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>84</v>
       </c>
@@ -995,7 +998,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>86</v>
       </c>
@@ -1006,7 +1009,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>69</v>
       </c>
@@ -1017,7 +1020,7 @@
         <v>3.75</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>57</v>
       </c>
@@ -1045,7 +1048,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>20</v>
       </c>
@@ -1073,7 +1076,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>22</v>
       </c>
@@ -1101,7 +1104,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>55</v>
       </c>
@@ -1129,7 +1132,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>71</v>
       </c>
@@ -1140,7 +1143,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>72</v>
       </c>
@@ -1151,7 +1154,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>73</v>
       </c>
@@ -1162,7 +1165,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>28</v>
       </c>
@@ -1190,7 +1193,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>40</v>
       </c>
@@ -1218,7 +1221,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>16</v>
       </c>
@@ -1229,7 +1232,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>10</v>
       </c>
@@ -1257,7 +1260,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>16</v>
       </c>
@@ -1285,7 +1288,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -1313,7 +1316,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>47</v>
       </c>
@@ -1341,7 +1344,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>51</v>
       </c>
@@ -1369,7 +1372,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>77</v>
       </c>
@@ -1380,7 +1383,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>7</v>
       </c>
@@ -1408,7 +1411,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>12</v>
       </c>
@@ -1436,7 +1439,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>14</v>
       </c>
@@ -1464,7 +1467,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>26</v>
       </c>
@@ -1492,7 +1495,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>30</v>
       </c>
@@ -1520,7 +1523,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>32</v>
       </c>
@@ -1548,7 +1551,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>36</v>
       </c>
@@ -1576,7 +1579,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>38</v>
       </c>
@@ -1604,7 +1607,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>42</v>
       </c>
@@ -1632,7 +1635,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>49</v>
       </c>
@@ -1660,7 +1663,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>75</v>
       </c>
@@ -1671,7 +1674,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>18</v>
       </c>
@@ -1699,7 +1702,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>53</v>
       </c>
@@ -1727,7 +1730,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>29</v>
       </c>
@@ -1749,7 +1752,7 @@
         <v>T</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>80</v>
       </c>
@@ -1771,7 +1774,7 @@
         <v>J</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>82</v>
       </c>
@@ -1793,7 +1796,7 @@
         <v>E</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>89</v>
       </c>
@@ -1815,7 +1818,7 @@
         <v>S</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>91</v>
       </c>
@@ -1837,7 +1840,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>93</v>
       </c>
@@ -1848,7 +1851,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>94</v>
       </c>
@@ -1859,7 +1862,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>91</v>
       </c>
@@ -1870,7 +1873,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>86</v>
       </c>
@@ -1881,7 +1884,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>98</v>
       </c>
@@ -1892,7 +1895,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>99</v>
       </c>
@@ -1903,7 +1906,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>100</v>
       </c>
@@ -1912,6 +1915,17 @@
       </c>
       <c r="C52">
         <v>1.5</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>93</v>
+      </c>
+      <c r="B53" t="s">
+        <v>102</v>
+      </c>
+      <c r="C53">
+        <v>4.5</v>
       </c>
     </row>
   </sheetData>
@@ -1930,9 +1944,9 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>87</v>
       </c>

</xml_diff>